<commit_message>
MS: date/time formatting using a R POSIX date/time formatter - dependency on joda time; removed setForceConversion and introduced additional the arguments forceConversion & dateTimeFormat in the readNamedRegion & readWorksheet calls
git-svn-id: svn://ms72.weblink.ch/mirai/XLConnect-R@181 ccc6e944-403e-a54a-b5f3-c2babcd103ea
</commit_message>
<xml_diff>
--- a/inst/demoFiles/conversion.xlsx
+++ b/inst/demoFiles/conversion.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>A</t>
   </si>
@@ -43,19 +43,25 @@
     <t>5</t>
   </si>
   <si>
-    <t>01/01/2012</t>
-  </si>
-  <si>
-    <t>01/28/2012</t>
-  </si>
-  <si>
     <t>TRUE</t>
   </si>
   <si>
     <t>FALSE</t>
   </si>
   <si>
-    <t>12/21/2012</t>
+    <t>2012-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2012-01-28 12:00:00</t>
+  </si>
+  <si>
+    <t>2012-12-21 12:45:15</t>
+  </si>
+  <si>
+    <t>2012-01-28 16:00:30</t>
+  </si>
+  <si>
+    <t>2012-01-01 21:15:00</t>
   </si>
 </sst>
 </file>
@@ -407,10 +413,13 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -428,10 +437,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -439,10 +448,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -453,7 +462,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -461,10 +470,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -472,10 +481,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>